<commit_message>
Update: add regular Expressions!
</commit_message>
<xml_diff>
--- a/static/uploads/dataTest_with_error.xlsx
+++ b/static/uploads/dataTest_with_error.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nico-\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\YoProgramo\python\Api_FastAPI\excel_validate\static\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACABC27-7ECC-4749-BCF5-AAB66EB90C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CB4A2E-5EC0-45CF-AA9C-35819392B0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="1515" windowWidth="21600" windowHeight="11835" xr2:uid="{FCE606B2-40F1-469F-A927-FD75F1CDBDAF}"/>
+    <workbookView xWindow="5655" yWindow="2115" windowWidth="21600" windowHeight="11835" xr2:uid="{FCE606B2-40F1-469F-A927-FD75F1CDBDAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -36,18 +36,12 @@
     <t>APELLIDO</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Martin</t>
   </si>
   <si>
     <t>Ramirez</t>
   </si>
   <si>
-    <t>adri@gmail.com</t>
-  </si>
-  <si>
     <t>Parra</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>mati22@outlook.com.ar</t>
-  </si>
-  <si>
     <t>Ramiro</t>
   </si>
   <si>
@@ -69,50 +60,101 @@
     <t>Romero</t>
   </si>
   <si>
-    <t>tincho77@hotmail.com</t>
-  </si>
-  <si>
-    <t>adri89@hotmail.com</t>
-  </si>
-  <si>
     <t>Adrian</t>
   </si>
   <si>
-    <t>Nicolas</t>
-  </si>
-  <si>
     <t>Alan</t>
   </si>
   <si>
     <t>Duarte</t>
   </si>
   <si>
-    <t>nico-po4@hotmail.com</t>
-  </si>
-  <si>
-    <t>tintin@outlook.com.ar</t>
-  </si>
-  <si>
-    <t>more@hotmail.com</t>
-  </si>
-  <si>
-    <t>matincho@outlook.com.ar</t>
-  </si>
-  <si>
-    <t>nico95@outlook.com.ar</t>
-  </si>
-  <si>
     <t>sdfs</t>
   </si>
   <si>
-    <t>456456@</t>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>institute</t>
+  </si>
+  <si>
+    <t>Harvard</t>
+  </si>
+  <si>
+    <t>san francisco</t>
+  </si>
+  <si>
+    <t>santa cat.</t>
+  </si>
+  <si>
+    <t>cuil</t>
+  </si>
+  <si>
+    <t>nico</t>
+  </si>
+  <si>
+    <t>86786_867867</t>
+  </si>
+  <si>
+    <t>85686786_786</t>
+  </si>
+  <si>
+    <t>867866_7867</t>
+  </si>
+  <si>
+    <t>86868-67868</t>
+  </si>
+  <si>
+    <t>5453_4753534</t>
+  </si>
+  <si>
+    <t>8678_6868</t>
+  </si>
+  <si>
+    <t>789_767667</t>
+  </si>
+  <si>
+    <t>86867-86786</t>
+  </si>
+  <si>
+    <t>686_6996657</t>
+  </si>
+  <si>
+    <t>3654_6346347</t>
+  </si>
+  <si>
+    <t>23433_453457</t>
+  </si>
+  <si>
+    <t>tini@gmail.com</t>
+  </si>
+  <si>
+    <t>ptifsdfni8@gmailcom</t>
+  </si>
+  <si>
+    <t>fsfrgmail.com</t>
+  </si>
+  <si>
+    <t>rami18@gmail.com</t>
+  </si>
+  <si>
+    <t>tinifsd@gmail.com</t>
+  </si>
+  <si>
+    <t>fsdf@hotmail</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>tinigmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,13 +172,6 @@
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -180,12 +215,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -502,19 +536,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C7BD24-0FE9-4293-9527-41ECC501086D}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,210 +563,312 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>3534</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2">
+        <v>453453</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3">
-        <v>21412</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>3534</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <v>4353</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>234</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>34534</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>345346</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5">
         <v>3534</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>234</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6">
+        <v>324</v>
+      </c>
+      <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="D7">
         <v>453453</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7">
+        <v>634</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="D8">
         <v>4353</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8">
+        <v>453453</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="D9">
         <v>34534</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9">
+        <v>4353</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10">
-        <v>3534</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10">
+        <v>43243534345</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="D11">
         <v>324</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11">
+        <v>3534</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12">
+      <c r="D12">
         <v>634</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12">
+        <v>324</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1" xr:uid="{898BB9A4-7EFF-4AB6-A5B4-FC49A59E17D4}"/>
-    <hyperlink ref="D11" r:id="rId2" xr:uid="{5E14FF77-6437-4793-B913-B48D6BBE4AD8}"/>
-    <hyperlink ref="D9" r:id="rId3" xr:uid="{1C6AB165-6D92-44B3-B1F9-C6B0AFB92CFD}"/>
-    <hyperlink ref="D8" r:id="rId4" xr:uid="{A03D9C25-38C7-41A0-90C7-A36D2F87D86D}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{812335B3-9916-40BE-B2E0-9B2654E95B25}"/>
-    <hyperlink ref="D6" r:id="rId6" xr:uid="{7018EDA3-86EA-4928-809E-9063CBC736FD}"/>
-    <hyperlink ref="D4" r:id="rId7" xr:uid="{1822FC40-8D6E-4CFC-881D-57AD2C5AF0C2}"/>
-    <hyperlink ref="D3" r:id="rId8" xr:uid="{3459446E-1568-4F33-BE39-1A5765B65AF6}"/>
-    <hyperlink ref="D2" r:id="rId9" xr:uid="{A29927D6-9CD0-45A7-B3DC-108486071F2D}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{E528D64A-654C-46C8-9739-B0522EC9D847}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{7A9C9346-1A9D-4CDC-BA9C-78D4028E001F}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{73DEC19A-D96A-4962-8A62-1ED7147B777D}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{C1C59F4B-D541-410B-840C-23F4805CBB18}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{6E414C2C-A10E-4EF7-8A1C-4D094BB705AE}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{2CFEBAF6-615E-4979-959A-843429EC3B27}"/>
+    <hyperlink ref="E11" r:id="rId6" xr:uid="{B84328D7-C9E9-44C7-8E0C-6365B13F26E9}"/>
+    <hyperlink ref="E7" r:id="rId7" xr:uid="{B0B23F54-E8AB-4BBE-A7AD-4E5303C35E90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>